<commit_message>
UI Format With Dept
</commit_message>
<xml_diff>
--- a/src/locale/i18n.xlsx
+++ b/src/locale/i18n.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mebugs\siteol\smart-ui\src\locale\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27945" windowHeight="12375" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="lang" sheetId="4" r:id="rId1"/>
     <sheet name="base" sheetId="1" r:id="rId2"/>
     <sheet name="plat" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="440">
   <si>
     <t>支持的语言列表（实际表格，按照顺序列填写文言）</t>
   </si>
@@ -775,10 +780,10 @@
     <t>response.code.sc</t>
   </si>
   <si>
-    <t>请输入响应码支持模糊查询</t>
-  </si>
-  <si>
-    <t>Please enter the response code to support fuzzy query</t>
+    <t>请输入响应码，支持模糊</t>
+  </si>
+  <si>
+    <t>Please enter the response code, fuzzy is supported</t>
   </si>
   <si>
     <t>response.zhCn</t>
@@ -787,7 +792,7 @@
     <t>汉语文言</t>
   </si>
   <si>
-    <t>Chinese classical Chinese</t>
+    <t>Chinese Classical Chinese</t>
   </si>
   <si>
     <t>response.zhCn.place</t>
@@ -805,7 +810,7 @@
     <t>英语文言</t>
   </si>
   <si>
-    <t>English classical Chinese</t>
+    <t>English Classical Chinese</t>
   </si>
   <si>
     <t>response.enUs.place</t>
@@ -823,7 +828,7 @@
     <t>响应备注</t>
   </si>
   <si>
-    <t>Response remarks</t>
+    <t>Response Remarks</t>
   </si>
   <si>
     <t>response.remark.place</t>
@@ -832,7 +837,7 @@
     <t>请输入响应备注信息</t>
   </si>
   <si>
-    <t>Please enter the response remarks</t>
+    <t>Please enter the response remark information</t>
   </si>
   <si>
     <t>response.del.tip</t>
@@ -841,7 +846,7 @@
     <t>锁定后响应码不可见但该响应码序号依旧保持占用！是否确认锁定？</t>
   </si>
   <si>
-    <t>After locking, the response code is invisible but the response code serial number remains occupied! Confirm the lock?</t>
+    <t>After locking, the response code is invisible but the response code number remains occupied! Confirm the lock?</t>
   </si>
   <si>
     <t>router.add</t>
@@ -892,10 +897,10 @@
     <t>router.url.sc</t>
   </si>
   <si>
-    <t>请输入接口地址支持模糊查询</t>
-  </si>
-  <si>
-    <t>Please enter the interface address. Fuzzy query is supported.</t>
+    <t>请输入接口地址，支持模糊</t>
+  </si>
+  <si>
+    <t>Please enter the interface address, support fuzzy</t>
   </si>
   <si>
     <t>router.url.format</t>
@@ -904,7 +909,7 @@
     <t>请输入合法的URL数据</t>
   </si>
   <si>
-    <t>Please enter a valid URL data.</t>
+    <t>Please enter a valid URL data</t>
   </si>
   <si>
     <t>router.url.place</t>
@@ -913,24 +918,18 @@
     <t>请输入URL需要以/开头例：/user/add</t>
   </si>
   <si>
-    <t>Please enter the URL. It must start with /. Example: /user/add</t>
+    <t>Please enter the URL, which must start with / Example: /user/add</t>
   </si>
   <si>
     <t>router.type</t>
   </si>
   <si>
-    <t>白名单路由</t>
-  </si>
-  <si>
     <t>Whitelist route</t>
   </si>
   <si>
     <t>router.type.tips</t>
   </si>
   <si>
-    <t>启用白名单路由则表示该路由无需授权即可访问</t>
-  </si>
-  <si>
     <t>Enabling whitelist route means that the route can be accessed without authorization</t>
   </si>
   <si>
@@ -946,19 +945,19 @@
     <t>router.name.sc</t>
   </si>
   <si>
-    <t>请输入路由名称支持模糊查询</t>
-  </si>
-  <si>
-    <t>Please enter the route name. Fuzzy query is supported.</t>
+    <t>请输入路由名称，支持模糊</t>
+  </si>
+  <si>
+    <t>Please enter the route name, support fuzzy</t>
   </si>
   <si>
     <t>router.name.place</t>
   </si>
   <si>
-    <t>请输入路由名称全局唯一</t>
-  </si>
-  <si>
-    <t>Please enter the route name. It is globally unique</t>
+    <t>请输入路由名称，全局唯一</t>
+  </si>
+  <si>
+    <t>Please enter the route name, which is globally unique</t>
   </si>
   <si>
     <t>router.logInDb</t>
@@ -1012,18 +1011,12 @@
     <t>请求报文中需要脱敏+Hash存储的字段该配置对入库和日志均生效</t>
   </si>
   <si>
-    <t>Fields in the request message that need to be desensitized + Hash storage. This configuration is effective for storage and log</t>
+    <t>Fields in the request message that need to be desensitized + Hash stored. This configuration is effective for both storage and log</t>
   </si>
   <si>
     <t>router.reqLogSecure.place</t>
   </si>
   <si>
-    <t>请输入字段名英文逗号分隔请勿输入回车例：namephone</t>
-  </si>
-  <si>
-    <t>Please enter the field name separated by commas in English. Do not enter the return key. Example: namephone</t>
-  </si>
-  <si>
     <t>router.resLogPrint</t>
   </si>
   <si>
@@ -1057,7 +1050,7 @@
     <t>响应报文中需要脱敏+Hash存储的字段该配置对入库和日志均生效</t>
   </si>
   <si>
-    <t>Fields in the response message that need to be desensitized + Hash storage. This configuration is effective for storage and log</t>
+    <t>Fields in the response message that need to be desensitized + Hash stored. This configuration is effective for both storage and log</t>
   </si>
   <si>
     <t>router.resLogSecure.place</t>
@@ -1078,16 +1071,16 @@
     <t>请输入路由备注信息</t>
   </si>
   <si>
-    <t>Please enter the route notes information</t>
+    <t>Please enter the route notes</t>
   </si>
   <si>
     <t>router.del.tip</t>
   </si>
   <si>
-    <t>删除路由后系统将拒绝该接口访问数据无法恢复是否确认删除改路由？</t>
-  </si>
-  <si>
-    <t>After deleting the route, the system will deny access to the interface. Data cannot be restored. Do you confirm to delete the route?</t>
+    <t>删除路由后系统将拒绝该接口访问，数据无法恢复，是否确认删除？</t>
+  </si>
+  <si>
+    <t>After deleting the route, the system will deny access to the interface, and the data cannot be restored. Do you confirm the deletion?</t>
   </si>
   <si>
     <t>permission.add.sub</t>
@@ -1096,7 +1089,7 @@
     <t>创建权限子集</t>
   </si>
   <si>
-    <t>Create permission subset</t>
+    <t>Create a permission subset</t>
   </si>
   <si>
     <t>permission.get</t>
@@ -1123,7 +1116,7 @@
     <t>同级权限排序</t>
   </si>
   <si>
-    <t>Permission sorting at the same level</t>
+    <t>Permission sorting for the same level</t>
   </si>
   <si>
     <t>permission.level</t>
@@ -1147,19 +1140,19 @@
     <t>permission.name.sc</t>
   </si>
   <si>
-    <t>请输入权限名称支持模糊</t>
-  </si>
-  <si>
-    <t>Please enter the permission name. Fuzzy is supported</t>
+    <t>请输入权限名称，支持模糊</t>
+  </si>
+  <si>
+    <t>Please enter the permission name, fuzzy is supported</t>
   </si>
   <si>
     <t>permission.name.place</t>
   </si>
   <si>
-    <t>请输入权限名称全局唯一</t>
-  </si>
-  <si>
-    <t>Please enter the permission name. Globally unique</t>
+    <t>请输入权限名称，全局唯一</t>
+  </si>
+  <si>
+    <t>Please enter the permission name, globally unique</t>
   </si>
   <si>
     <t>permission.alias</t>
@@ -1174,10 +1167,10 @@
     <t>permission.alias.place</t>
   </si>
   <si>
-    <t>请输入权限别名全局唯一</t>
-  </si>
-  <si>
-    <t>Please enter the permission alias. Globally unique</t>
+    <t>请输入权限别名，全局唯一</t>
+  </si>
+  <si>
+    <t>Please enter the permission alias, globally unique</t>
   </si>
   <si>
     <t>permission.static</t>
@@ -1219,23 +1212,155 @@
     <t>permission.del.tip</t>
   </si>
   <si>
-    <t>删除权限后相关访问将被拒绝数据无法恢复是否确认删除改权限？</t>
-  </si>
-  <si>
-    <t>After deleting a permission, the relevant access will be denied and the data cannot be recovered. Are you sure to delete the changed permission?</t>
+    <t>删除权限后相关访问将被拒绝，数据无法恢复，是否确认删除？</t>
+  </si>
+  <si>
+    <t>After deleting the permission, the relevant access will be denied and the data cannot be restored. Do you confirm the deletion?</t>
+  </si>
+  <si>
+    <t>role.add</t>
+  </si>
+  <si>
+    <t>创建角色</t>
+  </si>
+  <si>
+    <t>Create a role</t>
+  </si>
+  <si>
+    <t>role.add.sub</t>
+  </si>
+  <si>
+    <t>创建新的角色</t>
+  </si>
+  <si>
+    <t>Create a new role</t>
+  </si>
+  <si>
+    <t>role.get</t>
+  </si>
+  <si>
+    <t>查询角色</t>
+  </si>
+  <si>
+    <t>Query role</t>
+  </si>
+  <si>
+    <t>role.edit</t>
+  </si>
+  <si>
+    <t>编辑角色</t>
+  </si>
+  <si>
+    <t>Edit role</t>
+  </si>
+  <si>
+    <t>role.name</t>
+  </si>
+  <si>
+    <t>角色名称</t>
+  </si>
+  <si>
+    <t>Role name</t>
+  </si>
+  <si>
+    <t>role.name.sc</t>
+  </si>
+  <si>
+    <t>请输入角色名称，支持模糊</t>
+  </si>
+  <si>
+    <t>Please enter the role name, fuzzy is supported</t>
+  </si>
+  <si>
+    <t>role.name.place</t>
+  </si>
+  <si>
+    <t>请输入角色名称，全局唯一</t>
+  </si>
+  <si>
+    <t>Please enter the role name, globally unique</t>
+  </si>
+  <si>
+    <t>role.permissionIds</t>
+  </si>
+  <si>
+    <t>角色权限</t>
+  </si>
+  <si>
+    <t>Role permissions</t>
+  </si>
+  <si>
+    <t>role.permissionIds.tips</t>
+  </si>
+  <si>
+    <t>对于默认权限，即使没有选择也会默认赋予当前角色</t>
+  </si>
+  <si>
+    <t>For default permissions, the current role will be granted by default even if no selection is made</t>
+  </si>
+  <si>
+    <t>role.permissionIds.place</t>
+  </si>
+  <si>
+    <t>请在右侧权限树中勾选权限</t>
+  </si>
+  <si>
+    <t>Please check the permissions in the permission tree on the right</t>
+  </si>
+  <si>
+    <t>role.permissionIds.place.forGet</t>
+  </si>
+  <si>
+    <t>请在右侧查看角色具备的权限，包含默认权限</t>
+  </si>
+  <si>
+    <t>Please view the permissions that the role has on the right, including default permissions</t>
+  </si>
+  <si>
+    <t>role.remark</t>
+  </si>
+  <si>
+    <t>角色备注</t>
+  </si>
+  <si>
+    <t>Role notes</t>
+  </si>
+  <si>
+    <t>role.remark.place</t>
+  </si>
+  <si>
+    <t>请输入角色备注</t>
+  </si>
+  <si>
+    <t>Please enter the role notes</t>
+  </si>
+  <si>
+    <t>role.del.tip</t>
+  </si>
+  <si>
+    <t>删除角色后相关访问将被拒绝，数据无法恢复，是否确认删除？</t>
+  </si>
+  <si>
+    <t>After deleting the role, the relevant access will be denied and the data cannot be restored. Do you confirm the deletion?</t>
+  </si>
+  <si>
+    <t>请输入字段名英文逗号分隔请勿输入回车例：name,phone</t>
+  </si>
+  <si>
+    <t>Please enter the field name in English, separated by commas. Do not enter the return. Example: name,phone</t>
+  </si>
+  <si>
+    <t>路由类型</t>
+  </si>
+  <si>
+    <t>白名单路由则表示无需授权均可访问</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1254,346 +1379,16 @@
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1616,251 +1411,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1878,61 +1431,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2182,63 +1691,60 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B19:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="51.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" spans="1:1">
+    <row r="1" spans="1:1" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="17.25" spans="1:1">
+    <row r="2" spans="1:1" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="17.25" spans="1:1">
+    <row r="3" spans="1:1" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
       <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="37.375" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" spans="1:3">
+    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2249,7 +1755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="17.25" spans="1:3">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2260,7 +1766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="17.25" spans="1:3">
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2271,7 +1777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="17.25" spans="1:3">
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2282,7 +1788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" ht="17.25" spans="1:3">
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -2293,7 +1799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" ht="17.25" spans="1:3">
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -2304,7 +1810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" ht="17.25" spans="1:3">
+    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -2315,7 +1821,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" ht="17.25" spans="1:3">
+    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -2326,7 +1832,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" ht="17.25" spans="1:3">
+    <row r="9" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2337,7 +1843,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" ht="17.25" spans="1:3">
+    <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -2348,7 +1854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" ht="17.25" spans="1:3">
+    <row r="11" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
@@ -2359,7 +1865,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" ht="17.25" spans="1:3">
+    <row r="12" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -2370,7 +1876,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" ht="17.25" spans="1:3">
+    <row r="13" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -2381,7 +1887,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" ht="17.25" spans="1:3">
+    <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2392,7 +1898,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" ht="17.25" spans="1:3">
+    <row r="15" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
@@ -2403,7 +1909,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" ht="17.25" spans="1:3">
+    <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -2414,7 +1920,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" ht="17.25" spans="1:3">
+    <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -2425,7 +1931,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" ht="17.25" spans="1:3">
+    <row r="18" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>52</v>
       </c>
@@ -2436,7 +1942,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" ht="17.25" spans="1:3">
+    <row r="19" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
@@ -2447,7 +1953,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" ht="17.25" spans="1:3">
+    <row r="20" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>58</v>
       </c>
@@ -2458,7 +1964,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" ht="17.25" spans="1:3">
+    <row r="21" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>61</v>
       </c>
@@ -2469,7 +1975,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" ht="17.25" spans="1:3">
+    <row r="22" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>64</v>
       </c>
@@ -2480,7 +1986,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" ht="17.25" spans="1:3">
+    <row r="23" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>67</v>
       </c>
@@ -2491,7 +1997,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" ht="17.25" spans="1:3">
+    <row r="24" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>70</v>
       </c>
@@ -2502,7 +2008,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" ht="17.25" spans="1:3">
+    <row r="25" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
@@ -2513,7 +2019,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" ht="17.25" spans="1:3">
+    <row r="26" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -2524,7 +2030,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" ht="17.25" spans="1:3">
+    <row r="27" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -2535,7 +2041,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" ht="17.25" spans="1:3">
+    <row r="28" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -2546,7 +2052,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" ht="17.25" spans="1:3">
+    <row r="29" spans="1:3" ht="34.5" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>85</v>
       </c>
@@ -2557,7 +2063,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" ht="17.25" spans="1:3">
+    <row r="30" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>88</v>
       </c>
@@ -2568,7 +2074,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" ht="17.25" spans="1:3">
+    <row r="31" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>91</v>
       </c>
@@ -2579,7 +2085,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" ht="17.25" spans="1:3">
+    <row r="32" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>94</v>
       </c>
@@ -2590,7 +2096,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" ht="17.25" spans="1:3">
+    <row r="33" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>97</v>
       </c>
@@ -2601,7 +2107,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" ht="17.25" spans="1:3">
+    <row r="34" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>100</v>
       </c>
@@ -2612,7 +2118,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" ht="17.25" spans="1:3">
+    <row r="35" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>103</v>
       </c>
@@ -2623,7 +2129,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" ht="17.25" spans="1:3">
+    <row r="36" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>106</v>
       </c>
@@ -2634,7 +2140,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" ht="17.25" spans="1:3">
+    <row r="37" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>109</v>
       </c>
@@ -2648,29 +2154,26 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.375" customWidth="1"/>
+    <col min="1" max="1" width="29.875" customWidth="1"/>
     <col min="2" max="2" width="89.875" customWidth="1"/>
     <col min="3" max="3" width="173.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" spans="1:3">
+    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2681,7 +2184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="17.25" spans="1:3">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>112</v>
       </c>
@@ -2692,7 +2195,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" ht="17.25" spans="1:3">
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>115</v>
       </c>
@@ -2703,7 +2206,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" ht="17.25" spans="1:3">
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>118</v>
       </c>
@@ -2714,7 +2217,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" ht="17.25" spans="1:3">
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>121</v>
       </c>
@@ -2725,7 +2228,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" ht="17.25" spans="1:3">
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>124</v>
       </c>
@@ -2736,7 +2239,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" ht="17.25" spans="1:3">
+    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>127</v>
       </c>
@@ -2747,7 +2250,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" ht="17.25" spans="1:3">
+    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>130</v>
       </c>
@@ -2758,7 +2261,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" ht="17.25" spans="1:3">
+    <row r="9" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>133</v>
       </c>
@@ -2769,7 +2272,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" ht="17.25" spans="1:3">
+    <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>136</v>
       </c>
@@ -2780,7 +2283,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" ht="17.25" spans="1:3">
+    <row r="11" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>139</v>
       </c>
@@ -2791,7 +2294,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" ht="17.25" spans="1:3">
+    <row r="12" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>142</v>
       </c>
@@ -2802,7 +2305,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" ht="17.25" spans="1:3">
+    <row r="13" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>145</v>
       </c>
@@ -2813,7 +2316,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" ht="17.25" spans="1:3">
+    <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>148</v>
       </c>
@@ -2824,7 +2327,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" ht="17.25" spans="1:3">
+    <row r="15" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>151</v>
       </c>
@@ -2835,7 +2338,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" ht="17.25" spans="1:3">
+    <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>154</v>
       </c>
@@ -2846,7 +2349,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" ht="17.25" spans="1:3">
+    <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>157</v>
       </c>
@@ -2857,7 +2360,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" ht="17.25" spans="1:3">
+    <row r="18" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>160</v>
       </c>
@@ -2868,7 +2371,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" ht="17.25" spans="1:3">
+    <row r="19" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>163</v>
       </c>
@@ -2879,7 +2382,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" ht="17.25" spans="1:3">
+    <row r="20" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>166</v>
       </c>
@@ -2890,7 +2393,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" ht="17.25" spans="1:3">
+    <row r="21" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>169</v>
       </c>
@@ -2901,7 +2404,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="22" ht="17.25" spans="1:3">
+    <row r="22" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>172</v>
       </c>
@@ -2912,7 +2415,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="23" ht="17.25" spans="1:3">
+    <row r="23" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>175</v>
       </c>
@@ -2923,7 +2426,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" ht="17.25" spans="1:3">
+    <row r="24" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>178</v>
       </c>
@@ -2934,7 +2437,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" ht="17.25" spans="1:3">
+    <row r="25" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>181</v>
       </c>
@@ -2945,7 +2448,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="26" ht="17.25" spans="1:3">
+    <row r="26" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>184</v>
       </c>
@@ -2956,7 +2459,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27" ht="17.25" spans="1:3">
+    <row r="27" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>187</v>
       </c>
@@ -2967,7 +2470,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="28" ht="17.25" spans="1:3">
+    <row r="28" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>190</v>
       </c>
@@ -2978,7 +2481,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" ht="17.25" spans="1:3">
+    <row r="29" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>193</v>
       </c>
@@ -2989,7 +2492,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="30" ht="17.25" spans="1:3">
+    <row r="30" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>196</v>
       </c>
@@ -3000,7 +2503,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="31" ht="17.25" spans="1:3">
+    <row r="31" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>199</v>
       </c>
@@ -3011,7 +2514,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="32" ht="17.25" spans="1:3">
+    <row r="32" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>202</v>
       </c>
@@ -3022,7 +2525,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="33" ht="17.25" spans="1:3">
+    <row r="33" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>205</v>
       </c>
@@ -3033,7 +2536,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" ht="17.25" spans="1:3">
+    <row r="34" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>208</v>
       </c>
@@ -3044,7 +2547,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="35" ht="17.25" spans="1:3">
+    <row r="35" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>211</v>
       </c>
@@ -3055,7 +2558,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" ht="17.25" spans="1:3">
+    <row r="36" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>214</v>
       </c>
@@ -3066,7 +2569,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="37" ht="17.25" spans="1:3">
+    <row r="37" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>217</v>
       </c>
@@ -3077,7 +2580,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="38" ht="17.25" spans="1:3">
+    <row r="38" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>220</v>
       </c>
@@ -3088,7 +2591,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="39" ht="17.25" spans="1:3">
+    <row r="39" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>223</v>
       </c>
@@ -3099,7 +2602,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="40" ht="17.25" spans="1:3">
+    <row r="40" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>226</v>
       </c>
@@ -3110,7 +2613,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="41" ht="17.25" spans="1:3">
+    <row r="41" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>229</v>
       </c>
@@ -3121,7 +2624,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="42" ht="17.25" spans="1:3">
+    <row r="42" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>232</v>
       </c>
@@ -3132,7 +2635,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" ht="17.25" spans="1:3">
+    <row r="43" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>235</v>
       </c>
@@ -3143,7 +2646,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="44" ht="17.25" spans="1:3">
+    <row r="44" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>238</v>
       </c>
@@ -3154,7 +2657,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="45" ht="17.25" spans="1:3">
+    <row r="45" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>241</v>
       </c>
@@ -3165,7 +2668,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" ht="17.25" spans="1:3">
+    <row r="46" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>244</v>
       </c>
@@ -3176,7 +2679,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="47" ht="17.25" spans="1:3">
+    <row r="47" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>247</v>
       </c>
@@ -3187,7 +2690,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" ht="17.25" spans="1:3">
+    <row r="48" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>250</v>
       </c>
@@ -3198,7 +2701,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="49" ht="17.25" spans="1:3">
+    <row r="49" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>253</v>
       </c>
@@ -3209,7 +2712,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="50" ht="17.25" spans="1:3">
+    <row r="50" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
         <v>256</v>
       </c>
@@ -3220,7 +2723,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="51" ht="17.25" spans="1:3">
+    <row r="51" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
         <v>259</v>
       </c>
@@ -3231,7 +2734,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="52" ht="17.25" spans="1:3">
+    <row r="52" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>262</v>
       </c>
@@ -3242,7 +2745,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="53" ht="17.25" spans="1:3">
+    <row r="53" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>265</v>
       </c>
@@ -3253,7 +2756,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="54" ht="17.25" spans="1:3">
+    <row r="54" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>268</v>
       </c>
@@ -3264,7 +2767,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="55" ht="17.25" spans="1:3">
+    <row r="55" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
         <v>271</v>
       </c>
@@ -3275,7 +2778,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="56" ht="17.25" spans="1:3">
+    <row r="56" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
         <v>274</v>
       </c>
@@ -3286,7 +2789,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="57" ht="17.25" spans="1:3">
+    <row r="57" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
         <v>277</v>
       </c>
@@ -3297,7 +2800,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="58" ht="17.25" spans="1:3">
+    <row r="58" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
         <v>280</v>
       </c>
@@ -3308,7 +2811,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="59" ht="17.25" spans="1:3">
+    <row r="59" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
         <v>283</v>
       </c>
@@ -3319,7 +2822,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="60" ht="17.25" spans="1:3">
+    <row r="60" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
         <v>286</v>
       </c>
@@ -3330,7 +2833,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="61" ht="17.25" spans="1:3">
+    <row r="61" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>289</v>
       </c>
@@ -3341,7 +2844,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="62" ht="17.25" spans="1:3">
+    <row r="62" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
         <v>292</v>
       </c>
@@ -3352,394 +2855,547 @@
         <v>294</v>
       </c>
     </row>
-    <row r="63" ht="17.25" spans="1:3">
+    <row r="63" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
         <v>295</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C63" s="1" t="s">
+    </row>
+    <row r="64" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A64" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="64" ht="17.25" spans="1:3">
-      <c r="A64" s="2" t="s">
+      <c r="B64" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B64" s="1" t="s">
+    </row>
+    <row r="65" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A65" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="65" ht="17.25" spans="1:3">
-      <c r="A65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B65" s="1" t="s">
+    </row>
+    <row r="66" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A66" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="66" ht="17.25" spans="1:3">
-      <c r="A66" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B66" s="1" t="s">
+    </row>
+    <row r="67" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A67" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="67" ht="17.25" spans="1:3">
-      <c r="A67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B67" s="1" t="s">
+    </row>
+    <row r="68" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A68" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="68" ht="17.25" spans="1:3">
-      <c r="A68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B68" s="1" t="s">
+    </row>
+    <row r="69" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A69" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="69" ht="17.25" spans="1:3">
-      <c r="A69" s="2" t="s">
+      <c r="C69" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B69" s="1" t="s">
+    </row>
+    <row r="70" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A70" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="70" ht="17.25" spans="1:3">
-      <c r="A70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B70" s="1" t="s">
+    </row>
+    <row r="71" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A71" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="71" ht="17.25" spans="1:3">
-      <c r="A71" s="2" t="s">
+      <c r="C71" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B71" s="1" t="s">
+    </row>
+    <row r="72" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A72" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="72" ht="17.25" spans="1:3">
-      <c r="A72" s="2" t="s">
+      <c r="C72" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B72" s="1" t="s">
+    </row>
+    <row r="73" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A73" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="73" ht="17.25" spans="1:3">
-      <c r="A73" s="2" t="s">
+      <c r="C73" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B73" s="1" t="s">
+    </row>
+    <row r="74" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A74" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="B74" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A75" s="2" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="74" ht="17.25" spans="1:3">
-      <c r="A74" s="2" t="s">
+      <c r="B75" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C74" s="1" t="s">
+    </row>
+    <row r="76" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A76" s="2" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="75" ht="17.25" spans="1:3">
-      <c r="A75" s="2" t="s">
+      <c r="B76" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C75" s="1" t="s">
+    </row>
+    <row r="77" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A77" s="2" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="76" ht="17.25" spans="1:3">
-      <c r="A76" s="2" t="s">
+      <c r="B77" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C76" s="1" t="s">
+    </row>
+    <row r="78" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A78" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="77" ht="17.25" spans="1:3">
-      <c r="A77" s="2" t="s">
+      <c r="B78" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C77" s="1" t="s">
+    </row>
+    <row r="79" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A79" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="78" ht="17.25" spans="1:3">
-      <c r="A78" s="2" t="s">
+      <c r="B79" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A80" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="79" ht="17.25" spans="1:3">
-      <c r="A79" s="2" t="s">
+    <row r="81" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A81" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="80" ht="17.25" spans="1:3">
-      <c r="A80" s="2" t="s">
+      <c r="B81" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C80" s="1" t="s">
+    </row>
+    <row r="82" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A82" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="81" ht="17.25" spans="1:3">
-      <c r="A81" s="2" t="s">
+      <c r="B82" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C81" s="1" t="s">
+    </row>
+    <row r="83" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A83" s="2" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="82" ht="17.25" spans="1:3">
-      <c r="A82" s="2" t="s">
+      <c r="B83" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C82" s="1" t="s">
+    </row>
+    <row r="84" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A84" s="2" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="83" ht="17.25" spans="1:3">
-      <c r="A83" s="2" t="s">
+      <c r="B84" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="C83" s="1" t="s">
+    </row>
+    <row r="85" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A85" s="2" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="84" ht="17.25" spans="1:3">
-      <c r="A84" s="2" t="s">
+      <c r="B85" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C84" s="1" t="s">
+    </row>
+    <row r="86" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A86" s="2" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="85" ht="17.25" spans="1:3">
-      <c r="A85" s="2" t="s">
+      <c r="B86" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="C85" s="1" t="s">
+    </row>
+    <row r="87" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A87" s="2" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="86" ht="17.25" spans="1:3">
-      <c r="A86" s="2" t="s">
+      <c r="B87" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="C86" s="1" t="s">
+    </row>
+    <row r="88" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A88" s="2" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="87" ht="17.25" spans="1:3">
-      <c r="A87" s="2" t="s">
+      <c r="B88" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C87" s="1" t="s">
+    </row>
+    <row r="89" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A89" s="2" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="88" ht="17.25" spans="1:3">
-      <c r="A88" s="2" t="s">
+      <c r="B89" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="C88" s="1" t="s">
+    </row>
+    <row r="90" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A90" s="2" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="89" ht="17.25" spans="1:3">
-      <c r="A89" s="2" t="s">
+      <c r="B90" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="C89" s="1" t="s">
+    </row>
+    <row r="91" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A91" s="2" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="90" ht="17.25" spans="1:3">
-      <c r="A90" s="2" t="s">
+      <c r="B91" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C90" s="1" t="s">
+    </row>
+    <row r="92" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A92" s="2" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="91" ht="17.25" spans="1:3">
-      <c r="A91" s="2" t="s">
+      <c r="B92" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C91" s="1" t="s">
+    </row>
+    <row r="93" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A93" s="2" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="92" ht="17.25" spans="1:3">
-      <c r="A92" s="2" t="s">
+      <c r="B93" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C92" s="1" t="s">
+    </row>
+    <row r="94" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A94" s="2" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="93" ht="17.25" spans="1:3">
-      <c r="A93" s="2" t="s">
+      <c r="B94" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C93" s="1" t="s">
+    </row>
+    <row r="95" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A95" s="2" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="94" ht="17.25" spans="1:3">
-      <c r="A94" s="2" t="s">
+      <c r="B95" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C94" s="1" t="s">
+    </row>
+    <row r="96" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A96" s="2" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="95" ht="17.25" spans="1:3">
-      <c r="A95" s="2" t="s">
+      <c r="B96" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C95" s="1" t="s">
+    </row>
+    <row r="97" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A97" s="2" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="96" ht="17.25" spans="1:3">
-      <c r="A96" s="2" t="s">
+      <c r="B97" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="C96" s="1" t="s">
+    </row>
+    <row r="98" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A98" s="2" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="97" ht="17.25" spans="1:3">
-      <c r="A97" s="2" t="s">
+      <c r="B98" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C97" s="1" t="s">
+    </row>
+    <row r="99" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A99" s="2" t="s">
         <v>397</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A100" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A101" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A102" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A103" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A104" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A105" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A106" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A107" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="34.5" x14ac:dyDescent="0.15">
+      <c r="A108" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A109" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A110" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A111" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Plat Config V1 Fix
</commit_message>
<xml_diff>
--- a/src/locale/i18n.xlsx
+++ b/src/locale/i18n.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27945" windowHeight="12375" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27945" windowHeight="12375" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="lang" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="547">
   <si>
     <t>支持的语言列表（实际表格，按照顺序列填写文言）</t>
   </si>
@@ -1209,9 +1209,6 @@
     <t>Edit permission route set</t>
   </si>
   <si>
-    <t>permission.del.tip</t>
-  </si>
-  <si>
     <t>删除权限后相关访问将被拒绝，数据无法恢复，是否确认删除？</t>
   </si>
   <si>
@@ -1335,9 +1332,6 @@
     <t>Please enter the role notes</t>
   </si>
   <si>
-    <t>role.del.tip</t>
-  </si>
-  <si>
     <t>删除角色后相关访问将被拒绝，数据无法恢复，是否确认删除？</t>
   </si>
   <si>
@@ -1354,13 +1348,340 @@
   </si>
   <si>
     <t>白名单路由则表示无需授权均可访问</t>
+  </si>
+  <si>
+    <t>permission.del.tips</t>
+  </si>
+  <si>
+    <t>role.del.tips</t>
+  </si>
+  <si>
+    <t>dept.add.sub</t>
+  </si>
+  <si>
+    <t>dept.get</t>
+  </si>
+  <si>
+    <t>dept.edit</t>
+  </si>
+  <si>
+    <t>dept.name</t>
+  </si>
+  <si>
+    <t>dept.del.tips</t>
+  </si>
+  <si>
+    <t>dept.name.place</t>
+  </si>
+  <si>
+    <t>dept.permissionType</t>
+  </si>
+  <si>
+    <t>dept.permissionType.tips</t>
+  </si>
+  <si>
+    <t>dept.to</t>
+  </si>
+  <si>
+    <t>dept.sort</t>
+  </si>
+  <si>
+    <t>dept.toId</t>
+  </si>
+  <si>
+    <t>dept.toType</t>
+  </si>
+  <si>
+    <t>dept.toType.tips</t>
+  </si>
+  <si>
+    <t>dept.name.sc</t>
+  </si>
+  <si>
+    <t>创建子部门</t>
+  </si>
+  <si>
+    <t>查看部门</t>
+  </si>
+  <si>
+    <t>编辑部门</t>
+  </si>
+  <si>
+    <t>合并部门</t>
+  </si>
+  <si>
+    <t>目标部门</t>
+  </si>
+  <si>
+    <t>合并类型</t>
+  </si>
+  <si>
+    <t>合入：作为子部门加入目标部门；并入：成员和子部门加入目标部门。</t>
+  </si>
+  <si>
+    <t>同级部门排序</t>
+  </si>
+  <si>
+    <t>部门无账号以及子部门方可删除，您可通过部门合并转移相关数据。删除部门后，数据无法恢复，是否确认删除？</t>
+  </si>
+  <si>
+    <t>部门名称</t>
+  </si>
+  <si>
+    <t>请输入部门名称，全局唯一</t>
+  </si>
+  <si>
+    <t>请输入部门名称，支持模糊</t>
+  </si>
+  <si>
+    <t>数据权限类型</t>
+  </si>
+  <si>
+    <t>用于限制部门账号可以访问的数据范围，允许账号自定义</t>
+  </si>
+  <si>
+    <t>dept.accounts.isLeader</t>
+  </si>
+  <si>
+    <t>dept.accounts.unLeader</t>
+  </si>
+  <si>
+    <t>部门领导</t>
+  </si>
+  <si>
+    <t>部门成员</t>
+  </si>
+  <si>
+    <t>account.account</t>
+  </si>
+  <si>
+    <t>account.account.tips</t>
+  </si>
+  <si>
+    <t>account.account.place</t>
+  </si>
+  <si>
+    <t>account.permissionType</t>
+  </si>
+  <si>
+    <t>account.permissionType.tips</t>
+  </si>
+  <si>
+    <t>account.deptId</t>
+  </si>
+  <si>
+    <t>account.isLeader</t>
+  </si>
+  <si>
+    <t>account.status</t>
+  </si>
+  <si>
+    <t>account.name</t>
+  </si>
+  <si>
+    <t>account.name.place</t>
+  </si>
+  <si>
+    <t>account.roleIds</t>
+  </si>
+  <si>
+    <t>account.account.sc</t>
+  </si>
+  <si>
+    <t>account.name.sc</t>
+  </si>
+  <si>
+    <t>account.add</t>
+  </si>
+  <si>
+    <t>account.add.sub</t>
+  </si>
+  <si>
+    <t>account.get</t>
+  </si>
+  <si>
+    <t>account.edit</t>
+  </si>
+  <si>
+    <t>account.resetPwd</t>
+  </si>
+  <si>
+    <t>account.del.tips</t>
+  </si>
+  <si>
+    <t>account.resetPwd.tips</t>
+  </si>
+  <si>
+    <t>登陆账号</t>
+  </si>
+  <si>
+    <t>请输入登陆账号，全局唯一</t>
+  </si>
+  <si>
+    <t>请输入登陆账号，支持模糊</t>
+  </si>
+  <si>
+    <t>账号数据权限</t>
+  </si>
+  <si>
+    <t>用于限制登陆账号可以访问的数据范围，继承部门表示使用部门的配置</t>
+  </si>
+  <si>
+    <t>所属部门</t>
+  </si>
+  <si>
+    <t>部门职位</t>
+  </si>
+  <si>
+    <t>账号状态</t>
+  </si>
+  <si>
+    <t>个人姓名</t>
+  </si>
+  <si>
+    <t>请输入个人姓名，支持模糊</t>
+  </si>
+  <si>
+    <t>请输入个人姓名，全局唯一</t>
+  </si>
+  <si>
+    <t>绑定角色</t>
+  </si>
+  <si>
+    <t>创建账号</t>
+  </si>
+  <si>
+    <t>创建一个新账号</t>
+  </si>
+  <si>
+    <t>查看账号</t>
+  </si>
+  <si>
+    <t>编辑账号</t>
+  </si>
+  <si>
+    <t>重置密码</t>
+  </si>
+  <si>
+    <t>密码将被重置为123456，并在登陆需要用户再次重设密码</t>
+  </si>
+  <si>
+    <t>创建账号默认密码为123456，初次登陆需要用户重设密码</t>
+  </si>
+  <si>
+    <t>删除账号后，无法再次登陆且数据无法恢复，是否确认删除？</t>
+  </si>
+  <si>
+    <t>Create subdepartment</t>
+  </si>
+  <si>
+    <t>View department</t>
+  </si>
+  <si>
+    <t>Editorial Department</t>
+  </si>
+  <si>
+    <t>Merge departments</t>
+  </si>
+  <si>
+    <t>target department</t>
+  </si>
+  <si>
+    <t>Merge type</t>
+  </si>
+  <si>
+    <t>Sort by departments at the same level</t>
+  </si>
+  <si>
+    <t>Departments can be deleted only if they have no accounts and sub-departments. You can transfer relevant data through department merging. After deleting a department, the data cannot be recovered. Do you want to confirm the deletion?</t>
+  </si>
+  <si>
+    <t>Department name</t>
+  </si>
+  <si>
+    <t>Please enter a department name, it is globally unique</t>
+  </si>
+  <si>
+    <t>Please enter the department name, fuzzy is supported</t>
+  </si>
+  <si>
+    <t>Data permission type</t>
+  </si>
+  <si>
+    <t>Used to limit the data range that department accounts can access and allow account customization</t>
+  </si>
+  <si>
+    <t>Department heads</t>
+  </si>
+  <si>
+    <t>Department members</t>
+  </si>
+  <si>
+    <t>Login account</t>
+  </si>
+  <si>
+    <t>The default password when creating an account is 123456. The user needs to reset the password when logging in for the first time.</t>
+  </si>
+  <si>
+    <t>Please enter your login account, blur is supported</t>
+  </si>
+  <si>
+    <t>Please enter your login account, it is globally unique</t>
+  </si>
+  <si>
+    <t>Account data permissions</t>
+  </si>
+  <si>
+    <t>Department / Occupation</t>
+  </si>
+  <si>
+    <t>Account status</t>
+  </si>
+  <si>
+    <t>personal name</t>
+  </si>
+  <si>
+    <t>Please enter your personal name, blur is supported</t>
+  </si>
+  <si>
+    <t>Please enter your personal name, it is globally unique</t>
+  </si>
+  <si>
+    <t>Bind role</t>
+  </si>
+  <si>
+    <t>Create an account</t>
+  </si>
+  <si>
+    <t>Create a new account</t>
+  </si>
+  <si>
+    <t>View account</t>
+  </si>
+  <si>
+    <t>Edit account</t>
+  </si>
+  <si>
+    <t>reset Password</t>
+  </si>
+  <si>
+    <t>The password will be reset to 123456 and the user will be required to reset the password again upon login.</t>
+  </si>
+  <si>
+    <t>After deleting your account, you cannot log in again and the data cannot be recovered. Do you want to confirm the deletion?</t>
+  </si>
+  <si>
+    <t>Used to limit the data range that the login account can access. Inheriting the department means using the department\'s configuration.</t>
+  </si>
+  <si>
+    <t>Fit: Join the target department as a sub-department; Merge: Members and sub-departments join the target department.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1377,6 +1698,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -1417,7 +1744,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1428,6 +1755,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1732,14 +2065,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="37.375" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
   </cols>
@@ -2141,7 +2474,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2159,17 +2492,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.875" customWidth="1"/>
-    <col min="2" max="2" width="89.875" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="173.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2860,7 +3193,7 @@
         <v>295</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>296</v>
@@ -2871,7 +3204,7 @@
         <v>297</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>298</v>
@@ -2981,10 +3314,10 @@
         <v>326</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
@@ -3036,10 +3369,10 @@
         <v>339</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
@@ -3231,171 +3564,567 @@
     </row>
     <row r="97" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A97" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A98" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A99" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A100" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A101" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A102" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A103" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A104" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A105" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A106" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A107" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="C107" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="C107" s="1" t="s">
+    </row>
+    <row r="108" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A108" s="2" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" ht="34.5" x14ac:dyDescent="0.15">
-      <c r="A108" s="2" t="s">
+      <c r="B108" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A109" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
       <c r="A110" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="C110" s="1" t="s">
+    </row>
+    <row r="111" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A111" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B111" s="5" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
-      <c r="A111" s="2" t="s">
+      <c r="C111" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>435</v>
+    </row>
+    <row r="112" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A112" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A113" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A114" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A115" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A116" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A117" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A118" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A119" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A120" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A121" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A122" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A123" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A124" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A125" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A126" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A127" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A128" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A129" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A130" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A131" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A132" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A133" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A134" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A135" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A136" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A137" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A138" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A139" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A140" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A141" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A142" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A143" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A144" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A145" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A146" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="17.25" x14ac:dyDescent="0.15">
+      <c r="A147" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>544</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>